<commit_message>
:hotsprings: Fix Salary UI
</commit_message>
<xml_diff>
--- a/api/src/template/import_employee_template.xlsx
+++ b/api/src/template/import_employee_template.xlsx
@@ -186,13 +186,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -479,79 +479,79 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" style="1" customWidth="1"/>
-    <col min="14" max="15" width="17.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="18.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="17" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" style="2" customWidth="1"/>
+    <col min="14" max="15" width="17.140625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -559,52 +559,52 @@
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2" s="2">
         <v>100000</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="2" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
:hotsprings: Fix Salary UI (#126)
</commit_message>
<xml_diff>
--- a/api/src/template/import_employee_template.xlsx
+++ b/api/src/template/import_employee_template.xlsx
@@ -186,13 +186,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -479,79 +479,79 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" style="1" customWidth="1"/>
-    <col min="14" max="15" width="17.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="18.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="17" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" style="2" customWidth="1"/>
+    <col min="14" max="15" width="17.140625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -559,52 +559,52 @@
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2" s="2">
         <v>100000</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="2" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>